<commit_message>
1a versão apostila React
</commit_message>
<xml_diff>
--- a/curso/mysql/carro.xlsx
+++ b/curso/mysql/carro.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Carro" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Venda" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Cliente" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
   <si>
     <t xml:space="preserve">Marca</t>
   </si>
@@ -32,9 +33,30 @@
     <t xml:space="preserve">Ano de Lançamento</t>
   </si>
   <si>
+    <t xml:space="preserve">Cor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dat UltRevisão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Km</t>
+  </si>
+  <si>
     <t xml:space="preserve">Porsche</t>
   </si>
   <si>
+    <t xml:space="preserve">Vermelho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fiat</t>
   </si>
   <si>
@@ -119,7 +141,10 @@
     <t xml:space="preserve">Uno</t>
   </si>
   <si>
-    <t xml:space="preserve">Cliente</t>
+    <t xml:space="preserve">Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClienteId</t>
   </si>
   <si>
     <t xml:space="preserve">Vendedor</t>
@@ -134,109 +159,123 @@
     <t xml:space="preserve">Tel Cliente 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Valor Venda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forma de Pagamento</t>
+  </si>
+  <si>
     <t xml:space="preserve">Onix Plus</t>
   </si>
   <si>
+    <t xml:space="preserve">Carlos Almeida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(61) 92345-6789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(61) 92345-6700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renault</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwid Zen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana Paula Lima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(92) 99988-7766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creta Ultimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(43) 94567-8901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(43) 94567-8903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strada Freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(11) 91234-5678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corolla Cross</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro Costa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(41) 98765-4321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HB20 Platinum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(41) 98765-4320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR-V EXL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-Cross Comfortline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(31) 91122-3344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cronos Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juliana Barros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(71) 98765-1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(71) 98765-1235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(61) 92345-6780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome</t>
+  </si>
+  <si>
     <t xml:space="preserve">Carla Rodrigues</t>
   </si>
   <si>
-    <t xml:space="preserve">Carlos Almeida</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(61) 92345-6789</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(61) 92345-6700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renault</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kwid Zen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ana Paula Lima</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(92) 99988-7766</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creta Ultimate</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fernando Garcia</t>
   </si>
   <si>
-    <t xml:space="preserve">(43) 94567-8901</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(43) 94567-8903</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strada Freedom</t>
-  </si>
-  <si>
     <t xml:space="preserve">João Carlos Souza</t>
   </si>
   <si>
-    <t xml:space="preserve">(11) 91234-5678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corolla Cross</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maria Eduarda Silva</t>
   </si>
   <si>
-    <t xml:space="preserve">Pedro Costa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(41) 98765-4321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HB20 Platinum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(41) 98765-4320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR-V EXL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T-Cross Comfortline</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ricardo Nogueira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(31) 91122-3344</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cronos Drive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juliana Barros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(71) 98765-1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(71) 98765-1235</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -258,17 +297,20 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -313,36 +355,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -355,15 +401,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -478,31 +515,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.9"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>911</v>
@@ -510,126 +559,129 @@
       <c r="C2" s="3" t="n">
         <v>1963</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>1972</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>1966</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>1995</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>1976</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>1998</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>1938</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>1974</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>2012</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>1998</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>1979</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,86 +689,97 @@
         <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>2012</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>1964</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>2012</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>1968</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>1996</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>2013</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C20" s="3" t="n">
-        <v>1975</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="n">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="3" t="n">
         <v>1983</v>
       </c>
     </row>
@@ -736,254 +799,411 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="9.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="16.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="13.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="1" width="13.22"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="8" min="8" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>45799</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>45809</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>45813</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>45789</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>45797</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>45787</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>45792</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>45805</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>45795</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="6" t="n">
+        <v>45802</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="8" t="n">
+        <v>45821</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>24</v>
+      <c r="A2" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="6" t="n">
-        <v>45799</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>41</v>
+        <v>74</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>42</v>
+      <c r="A3" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="6" t="n">
-        <v>45809</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>17</v>
+      <c r="A4" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="6" t="n">
-        <v>45813</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>45789</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
+      <c r="A6" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>45797</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="6" t="n">
-        <v>45787</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="6" t="n">
-        <v>45792</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="B7" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="6" t="n">
-        <v>45805</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="6" t="n">
-        <v>45795</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="6" t="n">
-        <v>45802</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="B10" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>